<commit_message>
update with 3 omitted tracts
</commit_message>
<xml_diff>
--- a/data/brhd_le.xlsx
+++ b/data/brhd_le.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Equity Center/Github/brhd-vaccines/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mpc8t/Box Sync/mpc/dataForDemocracy/brhd/brhd-vaccines/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F5FAA4-7D63-5E42-9A61-67EE76E869CD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B855FF2-7238-F946-B7AE-78470C02A376}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{E34AF7FE-3C85-9945-A5AF-60BE9DEC46A1}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{E34AF7FE-3C85-9945-A5AF-60BE9DEC46A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="57">
   <si>
     <t xml:space="preserve"> Albemarle</t>
   </si>
@@ -184,6 +184,18 @@
   </si>
   <si>
     <t>Census Tract 7</t>
+  </si>
+  <si>
+    <t>Census Tract 102.02</t>
+  </si>
+  <si>
+    <t>Census Tract 109.01</t>
+  </si>
+  <si>
+    <t>Census Tract 109.02</t>
+  </si>
+  <si>
+    <t>Census Tract 109.03</t>
   </si>
 </sst>
 </file>
@@ -191,7 +203,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -279,11 +291,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -598,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39A644FA-4B8F-B44C-B7DD-49117B28D7AD}">
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="136" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1127,6 +1139,50 @@
         <v>81.89204264076993</v>
       </c>
     </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C48" s="11">
+        <v>85.876349582455006</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C49" s="8">
+        <v>81.601332669245451</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C50" s="11">
+        <v>81.272027683090585</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C51" s="8">
+        <v>85.150992842316668</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>